<commit_message>
[Localization + HeaderBar] complete feature Localization & header bar
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866072E0-2332-437F-8F80-CB6711010DA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37777D60-9984-456A-9ABD-21AD2994480C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>EN</t>
   </si>
@@ -46,16 +46,88 @@
     <t>KEY</t>
   </si>
   <si>
-    <t>txt_language</t>
-  </si>
-  <si>
-    <t>Việt Nam</t>
-  </si>
-  <si>
     <t>VN</t>
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>txt_language_vn</t>
+  </si>
+  <si>
+    <t>Tiếng Việt</t>
+  </si>
+  <si>
+    <t>Tiếng Anh</t>
+  </si>
+  <si>
+    <t>txt_language_en</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>txt_search</t>
+  </si>
+  <si>
+    <t>Tìm kiếm món ăn, địa điểm…</t>
+  </si>
+  <si>
+    <t>Find item, place, address…</t>
+  </si>
+  <si>
+    <t>txt_dish</t>
+  </si>
+  <si>
+    <t>Thức ăn</t>
+  </si>
+  <si>
+    <t>Dish</t>
+  </si>
+  <si>
+    <t>txt_login</t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>txt_order_history</t>
+  </si>
+  <si>
+    <t>Lịch sử đặt hàng</t>
+  </si>
+  <si>
+    <t>Order History</t>
+  </si>
+  <si>
+    <t>txt_my_vouchers</t>
+  </si>
+  <si>
+    <t>Khuyến mãi của tôi</t>
+  </si>
+  <si>
+    <t>txt_update_account</t>
+  </si>
+  <si>
+    <t>Cài đặt tài khoản</t>
+  </si>
+  <si>
+    <t>Update Account</t>
+  </si>
+  <si>
+    <t>My Vouchers</t>
+  </si>
+  <si>
+    <t>txt_logout</t>
+  </si>
+  <si>
+    <t>Đăng xuất</t>
+  </si>
+  <si>
+    <t>Log Out</t>
   </si>
 </sst>
 </file>
@@ -501,7 +573,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -526,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>0</v>
@@ -542,13 +614,13 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="15.6">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -560,9 +632,15 @@
       <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A3" s="4"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -573,9 +651,15 @@
       <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A4" s="4"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -586,9 +670,15 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A5" s="4"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -599,9 +689,15 @@
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A6" s="4"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -612,9 +708,15 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A7" s="4"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -625,9 +727,15 @@
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A8" s="4"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -638,9 +746,15 @@
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A9" s="4"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -651,9 +765,15 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A10" s="4"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>

</xml_diff>

<commit_message>
[Login] create UI component Login Page
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37777D60-9984-456A-9ABD-21AD2994480C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C335F83E-0270-447A-8159-E375B7A5FF97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>EN</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Đăng nhập</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>txt_order_history</t>
   </si>
   <si>
@@ -128,6 +125,54 @@
   </si>
   <si>
     <t>Log Out</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>txt_phone</t>
+  </si>
+  <si>
+    <t>Hoặc đăng nhập bằng tài khoản của bạn</t>
+  </si>
+  <si>
+    <t>Or sign in with your account</t>
+  </si>
+  <si>
+    <t>SỐ ĐIỆN THOẠI</t>
+  </si>
+  <si>
+    <t>PHONE NUMBER</t>
+  </si>
+  <si>
+    <t>txt_cacheSignIn</t>
+  </si>
+  <si>
+    <t>txt_optionSignIn</t>
+  </si>
+  <si>
+    <t>Lưu thông tin đăng nhập</t>
+  </si>
+  <si>
+    <t>txt_forgotPassword</t>
+  </si>
+  <si>
+    <t>Quên mật khẩu?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save login </t>
+  </si>
+  <si>
+    <t>Forgot password ?</t>
+  </si>
+  <si>
+    <t>txt_policy</t>
+  </si>
+  <si>
+    <t>We do not use your information for any purpose. By logging in or signing up, you agree with Foody's policies and regulations.</t>
+  </si>
+  <si>
+    <t>úng tôi không sử dụng thông tin của bạn với bất kỳ mục đích nào. Bằng cách đăng nhập hoặc đăng ký, bạn đồng ý với Chính sách quy định của Foody</t>
   </si>
 </sst>
 </file>
@@ -573,7 +618,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -696,7 +741,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
@@ -709,13 +754,13 @@
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="15.6">
       <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
@@ -728,13 +773,13 @@
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="15.6">
       <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
@@ -747,13 +792,13 @@
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" ht="15.6">
       <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
@@ -766,13 +811,13 @@
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" ht="15.6">
       <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
@@ -784,9 +829,15 @@
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A11" s="4"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -797,9 +848,15 @@
       <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -810,9 +867,15 @@
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A13" s="4"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -823,9 +886,15 @@
       <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A14" s="4"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -835,10 +904,16 @@
       <c r="J14" s="10"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A15" s="4"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="4"/>
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="45">
+      <c r="A15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>

</xml_diff>

<commit_message>
[Login/ HomePage] create fb & gg app id, create homepage index
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C335F83E-0270-447A-8159-E375B7A5FF97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1467F55E-07B4-4D12-90CB-0615D3A794B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
   <si>
     <t>EN</t>
   </si>
@@ -174,12 +174,157 @@
   <si>
     <t>úng tôi không sử dụng thông tin của bạn với bất kỳ mục đích nào. Bằng cách đăng nhập hoặc đăng ký, bạn đồng ý với Chính sách quy định của Foody</t>
   </si>
+  <si>
+    <t>title_order_homepage</t>
+  </si>
+  <si>
+    <t>Đặt Đồ ăn, giao hàng từ 20'…</t>
+  </si>
+  <si>
+    <t>title_order_intro_homepage</t>
+  </si>
+  <si>
+    <t>Có @num Địa Điểm Ở @area Từ 00:00 - 23:59</t>
+  </si>
+  <si>
+    <t>txt_gui_download_app</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_0</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_1</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_2</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_3</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_4</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_5</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_6</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_7</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_8</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_9</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_10</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_11</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_12</t>
+  </si>
+  <si>
+    <t>txt_type_food_homepage_13</t>
+  </si>
+  <si>
+    <t>Đồ ăn</t>
+  </si>
+  <si>
+    <t>Đồ uống</t>
+  </si>
+  <si>
+    <t>Đồ chay</t>
+  </si>
+  <si>
+    <t>Bánh kem</t>
+  </si>
+  <si>
+    <t>Tráng miệng</t>
+  </si>
+  <si>
+    <t>Homemade</t>
+  </si>
+  <si>
+    <t>Vỉa hè</t>
+  </si>
+  <si>
+    <t>Pizza/ Burger</t>
+  </si>
+  <si>
+    <t>Món gà</t>
+  </si>
+  <si>
+    <t>Món lẩu</t>
+  </si>
+  <si>
+    <t>Sushi</t>
+  </si>
+  <si>
+    <t>Mì phở</t>
+  </si>
+  <si>
+    <t>Cơm hộp</t>
+  </si>
+  <si>
+    <t>Order Food, delivery from 20'…</t>
+  </si>
+  <si>
+    <t>From @num Places In @area From 00:00 - 23:59</t>
+  </si>
+  <si>
+    <t>Better experiences with Flash App</t>
+  </si>
+  <si>
+    <t>Tất cả</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Drink</t>
+  </si>
+  <si>
+    <t>Vege</t>
+  </si>
+  <si>
+    <t>Cakes</t>
+  </si>
+  <si>
+    <t>Dessert</t>
+  </si>
+  <si>
+    <t>Streetfood</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Hotpot</t>
+  </si>
+  <si>
+    <t>Noodles</t>
+  </si>
+  <si>
+    <t>Rice box</t>
+  </si>
+  <si>
+    <t>Sử dụng App Flash để có nhiều giảm giá \n
+và trải nghiệm tốt hơn</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +393,12 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -615,10 +766,10 @@
   <dimension ref="A1:K1082"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8"/>
@@ -924,9 +1075,15 @@
       <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A16" s="4"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -937,9 +1094,15 @@
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A17" s="4"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -949,10 +1112,16 @@
       <c r="J17" s="10"/>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A18" s="4"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="4"/>
+    <row r="18" spans="1:11" s="2" customFormat="1" ht="30">
+      <c r="A18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -963,9 +1132,15 @@
       <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A19" s="4"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="4"/>
+      <c r="A19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -976,9 +1151,15 @@
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A20" s="4"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -989,9 +1170,15 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A21" s="4"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1002,9 +1189,15 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A22" s="4"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1015,9 +1208,15 @@
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A23" s="4"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1028,9 +1227,15 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A24" s="4"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1041,9 +1246,15 @@
       <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A25" s="4"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="4"/>
+      <c r="A25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1054,9 +1265,15 @@
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A26" s="4"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="4"/>
+      <c r="A26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1067,9 +1284,15 @@
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A27" s="4"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1080,9 +1303,15 @@
       <c r="K27" s="11"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A28" s="4"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1093,9 +1322,15 @@
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A29" s="4"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="4"/>
+      <c r="A29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1106,9 +1341,15 @@
       <c r="K29" s="11"/>
     </row>
     <row r="30" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A30" s="4"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="4"/>
+      <c r="A30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1119,9 +1360,15 @@
       <c r="K30" s="11"/>
     </row>
     <row r="31" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A31" s="4"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="4"/>
+      <c r="A31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1132,9 +1379,15 @@
       <c r="K31" s="11"/>
     </row>
     <row r="32" spans="1:11" s="2" customFormat="1" ht="15.6">
-      <c r="A32" s="4"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -14764,6 +15017,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I673" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[NotFoundPage] add 404 page & set up notify no-result-found in filter restaurants
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EF1DE4-6525-4B9D-B0A8-7F518601D1CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A0EEFE-7112-4F9A-9BB9-B097C9A1B9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$673</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$674</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="200">
   <si>
     <t>EN</t>
   </si>
@@ -621,6 +621,24 @@
   </si>
   <si>
     <t>Loại</t>
+  </si>
+  <si>
+    <t>txt_no_result_found</t>
+  </si>
+  <si>
+    <t>Không tìm thấy kết quả tìm kiếm!</t>
+  </si>
+  <si>
+    <t>No search results found!</t>
+  </si>
+  <si>
+    <t>txt_district_24</t>
+  </si>
+  <si>
+    <t>Gò vấp</t>
+  </si>
+  <si>
+    <t>Go Vap</t>
   </si>
 </sst>
 </file>
@@ -1066,13 +1084,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K1082"/>
+  <dimension ref="A1:K1083"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -2253,13 +2271,13 @@
     </row>
     <row r="62" spans="1:11" s="2" customFormat="1">
       <c r="A62" s="4" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
@@ -2272,13 +2290,13 @@
     </row>
     <row r="63" spans="1:11" s="2" customFormat="1">
       <c r="A63" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
@@ -2291,13 +2309,13 @@
     </row>
     <row r="64" spans="1:11" s="2" customFormat="1">
       <c r="A64" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>82</v>
+        <v>182</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
@@ -2310,13 +2328,13 @@
     </row>
     <row r="65" spans="1:11" s="2" customFormat="1">
       <c r="A65" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
@@ -2329,13 +2347,13 @@
     </row>
     <row r="66" spans="1:11" s="2" customFormat="1">
       <c r="A66" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>190</v>
+        <v>66</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
@@ -2348,13 +2366,13 @@
     </row>
     <row r="67" spans="1:11" s="2" customFormat="1">
       <c r="A67" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
@@ -2367,13 +2385,13 @@
     </row>
     <row r="68" spans="1:11" s="2" customFormat="1">
       <c r="A68" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>74</v>
+        <v>191</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="4"/>
@@ -2386,13 +2404,13 @@
     </row>
     <row r="69" spans="1:11" s="2" customFormat="1">
       <c r="A69" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>183</v>
+        <v>188</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>183</v>
+        <v>89</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
@@ -2405,13 +2423,13 @@
     </row>
     <row r="70" spans="1:11" s="2" customFormat="1">
       <c r="A70" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>73</v>
+        <v>189</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>88</v>
+        <v>183</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
@@ -2423,9 +2441,15 @@
       <c r="K70" s="11"/>
     </row>
     <row r="71" spans="1:11" s="2" customFormat="1">
-      <c r="A71" s="4"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="4"/>
+      <c r="A71" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="D71" s="3"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -2436,9 +2460,15 @@
       <c r="K71" s="11"/>
     </row>
     <row r="72" spans="1:11" s="2" customFormat="1">
-      <c r="A72" s="4"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="4"/>
+      <c r="A72" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="D72" s="3"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -15526,10 +15556,18 @@
       <c r="J1078" s="10"/>
       <c r="K1078" s="11"/>
     </row>
-    <row r="1079" spans="1:11">
-      <c r="A1079" s="8"/>
-      <c r="B1079" s="8"/>
-      <c r="C1079" s="8"/>
+    <row r="1079" spans="1:11" s="2" customFormat="1">
+      <c r="A1079" s="4"/>
+      <c r="B1079" s="7"/>
+      <c r="C1079" s="4"/>
+      <c r="D1079" s="3"/>
+      <c r="E1079" s="4"/>
+      <c r="F1079" s="4"/>
+      <c r="G1079" s="4"/>
+      <c r="H1079" s="4"/>
+      <c r="I1079" s="4"/>
+      <c r="J1079" s="10"/>
+      <c r="K1079" s="11"/>
     </row>
     <row r="1080" spans="1:11">
       <c r="A1080" s="8"/>
@@ -15546,8 +15584,13 @@
       <c r="B1082" s="8"/>
       <c r="C1082" s="8"/>
     </row>
+    <row r="1083" spans="1:11">
+      <c r="A1083" s="8"/>
+      <c r="B1083" s="8"/>
+      <c r="C1083" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I673" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I674" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
localize page VertifyPhone & Input OTP, add fake service
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A0EEFE-7112-4F9A-9BB9-B097C9A1B9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3414B9F-CA3E-4558-A933-A669BB89393E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="215">
   <si>
     <t>EN</t>
   </si>
@@ -639,6 +639,51 @@
   </si>
   <si>
     <t>Go Vap</t>
+  </si>
+  <si>
+    <t>txt_invalid_otp</t>
+  </si>
+  <si>
+    <t>Mã OTP không hợp lệ</t>
+  </si>
+  <si>
+    <t>The OTP is invalid</t>
+  </si>
+  <si>
+    <t>txt_confirm</t>
+  </si>
+  <si>
+    <t>Xác nhận</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>txt_enter_otp</t>
+  </si>
+  <si>
+    <t>Nhập mã OTP</t>
+  </si>
+  <si>
+    <t>Enter OTP</t>
+  </si>
+  <si>
+    <t>txt_vertify_phone_number</t>
+  </si>
+  <si>
+    <t>Xác thực số điện thoại</t>
+  </si>
+  <si>
+    <t>Vertify Phone Number</t>
+  </si>
+  <si>
+    <t>txt_your_phone_number</t>
+  </si>
+  <si>
+    <t>Số điện thoại của bạn</t>
+  </si>
+  <si>
+    <t>Your phone number</t>
   </si>
 </sst>
 </file>
@@ -1087,10 +1132,10 @@
   <dimension ref="A1:K1083"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
+      <selection pane="bottomRight" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -2479,9 +2524,15 @@
       <c r="K72" s="11"/>
     </row>
     <row r="73" spans="1:11" s="2" customFormat="1">
-      <c r="A73" s="4"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="4"/>
+      <c r="A73" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>202</v>
+      </c>
       <c r="D73" s="3"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -2492,9 +2543,15 @@
       <c r="K73" s="11"/>
     </row>
     <row r="74" spans="1:11" s="2" customFormat="1">
-      <c r="A74" s="4"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="4"/>
+      <c r="A74" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>205</v>
+      </c>
       <c r="D74" s="3"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -2505,9 +2562,15 @@
       <c r="K74" s="11"/>
     </row>
     <row r="75" spans="1:11" s="2" customFormat="1">
-      <c r="A75" s="4"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="4"/>
+      <c r="A75" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>208</v>
+      </c>
       <c r="D75" s="3"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -2518,9 +2581,15 @@
       <c r="K75" s="11"/>
     </row>
     <row r="76" spans="1:11" s="2" customFormat="1">
-      <c r="A76" s="4"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="4"/>
+      <c r="A76" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="D76" s="3"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -2531,9 +2600,15 @@
       <c r="K76" s="11"/>
     </row>
     <row r="77" spans="1:11" s="2" customFormat="1">
-      <c r="A77" s="4"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="4"/>
+      <c r="A77" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="D77" s="3"/>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>

</xml_diff>

<commit_message>
[API] optimize flow network (fake API) for SignIn & ListRestaurant
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3414B9F-CA3E-4558-A933-A669BB89393E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149F2E92-AA89-46DD-9CEE-4DDFE582C4D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="236">
   <si>
     <t>EN</t>
   </si>
@@ -684,6 +684,69 @@
   </si>
   <si>
     <t>Your phone number</t>
+  </si>
+  <si>
+    <t>txt_preferred</t>
+  </si>
+  <si>
+    <t>Yêu thích</t>
+  </si>
+  <si>
+    <t>Preferred</t>
+  </si>
+  <si>
+    <t>txt_open</t>
+  </si>
+  <si>
+    <t>txt_closed</t>
+  </si>
+  <si>
+    <t>txt_closed_soon</t>
+  </si>
+  <si>
+    <t>Đang mở cửa</t>
+  </si>
+  <si>
+    <t>Đóng cửa</t>
+  </si>
+  <si>
+    <t>Sắp đóng cửa</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Close soon</t>
+  </si>
+  <si>
+    <t>txt_wrong_signin</t>
+  </si>
+  <si>
+    <t>Thông tin đăng nhập không chính xác</t>
+  </si>
+  <si>
+    <t>Sign in information is incorrect</t>
+  </si>
+  <si>
+    <t>txt_phone_number_used</t>
+  </si>
+  <si>
+    <t>Số điện thoại đã được sử dụng</t>
+  </si>
+  <si>
+    <t>Số điện thoại không đúng định dạng</t>
+  </si>
+  <si>
+    <t>txt_invalid_phone_number</t>
+  </si>
+  <si>
+    <t>Phone number already in use</t>
+  </si>
+  <si>
+    <t>Phone number is not in the correct format</t>
   </si>
 </sst>
 </file>
@@ -1132,10 +1195,10 @@
   <dimension ref="A1:K1083"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A76" sqref="A76"/>
+      <selection pane="bottomRight" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -2619,9 +2682,15 @@
       <c r="K77" s="11"/>
     </row>
     <row r="78" spans="1:11" s="2" customFormat="1">
-      <c r="A78" s="4"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="4"/>
+      <c r="A78" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="D78" s="3"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -2632,9 +2701,15 @@
       <c r="K78" s="11"/>
     </row>
     <row r="79" spans="1:11" s="2" customFormat="1">
-      <c r="A79" s="4"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="4"/>
+      <c r="A79" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>224</v>
+      </c>
       <c r="D79" s="3"/>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -2645,9 +2720,15 @@
       <c r="K79" s="11"/>
     </row>
     <row r="80" spans="1:11" s="2" customFormat="1">
-      <c r="A80" s="4"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="4"/>
+      <c r="A80" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>225</v>
+      </c>
       <c r="D80" s="3"/>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
@@ -2658,9 +2739,15 @@
       <c r="K80" s="11"/>
     </row>
     <row r="81" spans="1:11" s="2" customFormat="1">
-      <c r="A81" s="4"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="4"/>
+      <c r="A81" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="D81" s="3"/>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
@@ -2671,9 +2758,15 @@
       <c r="K81" s="11"/>
     </row>
     <row r="82" spans="1:11" s="2" customFormat="1">
-      <c r="A82" s="4"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="4"/>
+      <c r="A82" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>229</v>
+      </c>
       <c r="D82" s="3"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
@@ -2684,9 +2777,15 @@
       <c r="K82" s="11"/>
     </row>
     <row r="83" spans="1:11" s="2" customFormat="1">
-      <c r="A83" s="4"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="4"/>
+      <c r="A83" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>234</v>
+      </c>
       <c r="D83" s="3"/>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
@@ -2697,9 +2796,15 @@
       <c r="K83" s="11"/>
     </row>
     <row r="84" spans="1:11" s="2" customFormat="1">
-      <c r="A84" s="4"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="4"/>
+      <c r="A84" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>235</v>
+      </c>
       <c r="D84" s="3"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>

</xml_diff>

<commit_message>
[Profile] create side bar with behavior
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149F2E92-AA89-46DD-9CEE-4DDFE582C4D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047C78DB-5AB1-464F-BCC1-D9A241957035}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="247">
   <si>
     <t>EN</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>txt_update_account</t>
-  </si>
-  <si>
-    <t>Cài đặt tài khoản</t>
   </si>
   <si>
     <t>Update Account</t>
@@ -747,6 +744,42 @@
   </si>
   <si>
     <t>Phone number is not in the correct format</t>
+  </si>
+  <si>
+    <t>txt_submit</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>txt_input_your_phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhập số điện thoại </t>
+  </si>
+  <si>
+    <t>Input your phone number</t>
+  </si>
+  <si>
+    <t>txt_resend_otp</t>
+  </si>
+  <si>
+    <t>Gửi lại mã OTP</t>
+  </si>
+  <si>
+    <t>Resend OTP</t>
+  </si>
+  <si>
+    <t>Cập nhập tài khoản</t>
+  </si>
+  <si>
+    <t>txt_payment_type</t>
+  </si>
+  <si>
+    <t>Phương thức thanh toán</t>
+  </si>
+  <si>
+    <t>Payment methods</t>
   </si>
 </sst>
 </file>
@@ -1195,10 +1228,10 @@
   <dimension ref="A1:K1083"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B73" sqref="B73"/>
+      <selection pane="bottomRight" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -1321,7 +1354,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
@@ -1359,7 +1392,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
@@ -1375,10 +1408,10 @@
         <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
@@ -1391,13 +1424,13 @@
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1">
       <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
@@ -1410,13 +1443,13 @@
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
@@ -1429,13 +1462,13 @@
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
@@ -1448,13 +1481,13 @@
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1">
       <c r="A13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
@@ -1467,13 +1500,13 @@
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1">
       <c r="A14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
@@ -1486,13 +1519,13 @@
     </row>
     <row r="15" spans="1:11" s="2" customFormat="1" ht="42.75">
       <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
@@ -1505,13 +1538,13 @@
     </row>
     <row r="16" spans="1:11" s="2" customFormat="1">
       <c r="A16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
@@ -1524,13 +1557,13 @@
     </row>
     <row r="17" spans="1:11" s="2" customFormat="1">
       <c r="A17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="C17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
@@ -1543,13 +1576,13 @@
     </row>
     <row r="18" spans="1:11" s="2" customFormat="1" ht="28.5">
       <c r="A18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
@@ -1562,13 +1595,13 @@
     </row>
     <row r="19" spans="1:11" s="2" customFormat="1">
       <c r="A19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
@@ -1581,13 +1614,13 @@
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1">
       <c r="A20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
@@ -1600,13 +1633,13 @@
     </row>
     <row r="21" spans="1:11" s="2" customFormat="1">
       <c r="A21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
@@ -1619,13 +1652,13 @@
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1">
       <c r="A22" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
@@ -1638,13 +1671,13 @@
     </row>
     <row r="23" spans="1:11" s="2" customFormat="1">
       <c r="A23" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
@@ -1657,13 +1690,13 @@
     </row>
     <row r="24" spans="1:11" s="2" customFormat="1">
       <c r="A24" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
@@ -1676,13 +1709,13 @@
     </row>
     <row r="25" spans="1:11" s="2" customFormat="1">
       <c r="A25" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
@@ -1695,13 +1728,13 @@
     </row>
     <row r="26" spans="1:11" s="2" customFormat="1">
       <c r="A26" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
@@ -1714,13 +1747,13 @@
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1">
       <c r="A27" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
@@ -1733,13 +1766,13 @@
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1">
       <c r="A28" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
@@ -1752,13 +1785,13 @@
     </row>
     <row r="29" spans="1:11" s="2" customFormat="1">
       <c r="A29" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
@@ -1771,13 +1804,13 @@
     </row>
     <row r="30" spans="1:11" s="2" customFormat="1">
       <c r="A30" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
@@ -1790,13 +1823,13 @@
     </row>
     <row r="31" spans="1:11" s="2" customFormat="1">
       <c r="A31" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
@@ -1809,13 +1842,13 @@
     </row>
     <row r="32" spans="1:11" s="2" customFormat="1">
       <c r="A32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
@@ -1828,13 +1861,13 @@
     </row>
     <row r="33" spans="1:11" s="2" customFormat="1">
       <c r="A33" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
@@ -1847,13 +1880,13 @@
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1">
       <c r="A34" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
@@ -1866,13 +1899,13 @@
     </row>
     <row r="35" spans="1:11" s="2" customFormat="1">
       <c r="A35" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
@@ -1885,13 +1918,13 @@
     </row>
     <row r="36" spans="1:11" s="2" customFormat="1">
       <c r="A36" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
@@ -1904,13 +1937,13 @@
     </row>
     <row r="37" spans="1:11" s="2" customFormat="1">
       <c r="A37" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="C37" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
@@ -1923,13 +1956,13 @@
     </row>
     <row r="38" spans="1:11" s="2" customFormat="1">
       <c r="A38" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="C38" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
@@ -1942,13 +1975,13 @@
     </row>
     <row r="39" spans="1:11" s="2" customFormat="1">
       <c r="A39" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
@@ -1961,13 +1994,13 @@
     </row>
     <row r="40" spans="1:11" s="2" customFormat="1">
       <c r="A40" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
@@ -1980,13 +2013,13 @@
     </row>
     <row r="41" spans="1:11" s="2" customFormat="1">
       <c r="A41" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
@@ -1999,13 +2032,13 @@
     </row>
     <row r="42" spans="1:11" s="2" customFormat="1">
       <c r="A42" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
@@ -2018,13 +2051,13 @@
     </row>
     <row r="43" spans="1:11" s="2" customFormat="1">
       <c r="A43" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
@@ -2037,13 +2070,13 @@
     </row>
     <row r="44" spans="1:11" s="2" customFormat="1">
       <c r="A44" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
@@ -2056,13 +2089,13 @@
     </row>
     <row r="45" spans="1:11" s="2" customFormat="1">
       <c r="A45" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
@@ -2075,13 +2108,13 @@
     </row>
     <row r="46" spans="1:11" s="2" customFormat="1">
       <c r="A46" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
@@ -2094,13 +2127,13 @@
     </row>
     <row r="47" spans="1:11" s="2" customFormat="1">
       <c r="A47" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
@@ -2113,13 +2146,13 @@
     </row>
     <row r="48" spans="1:11" s="2" customFormat="1">
       <c r="A48" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
@@ -2132,13 +2165,13 @@
     </row>
     <row r="49" spans="1:11" s="2" customFormat="1">
       <c r="A49" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="4"/>
@@ -2151,13 +2184,13 @@
     </row>
     <row r="50" spans="1:11" s="2" customFormat="1">
       <c r="A50" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="4"/>
@@ -2170,13 +2203,13 @@
     </row>
     <row r="51" spans="1:11" s="2" customFormat="1">
       <c r="A51" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="4"/>
@@ -2189,13 +2222,13 @@
     </row>
     <row r="52" spans="1:11" s="2" customFormat="1">
       <c r="A52" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
@@ -2208,13 +2241,13 @@
     </row>
     <row r="53" spans="1:11" s="2" customFormat="1">
       <c r="A53" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="4"/>
@@ -2227,13 +2260,13 @@
     </row>
     <row r="54" spans="1:11" s="2" customFormat="1">
       <c r="A54" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="4"/>
@@ -2246,13 +2279,13 @@
     </row>
     <row r="55" spans="1:11" s="2" customFormat="1">
       <c r="A55" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="4"/>
@@ -2265,13 +2298,13 @@
     </row>
     <row r="56" spans="1:11" s="2" customFormat="1">
       <c r="A56" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="4"/>
@@ -2284,13 +2317,13 @@
     </row>
     <row r="57" spans="1:11" s="2" customFormat="1">
       <c r="A57" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="4"/>
@@ -2303,13 +2336,13 @@
     </row>
     <row r="58" spans="1:11" s="2" customFormat="1">
       <c r="A58" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="4"/>
@@ -2322,13 +2355,13 @@
     </row>
     <row r="59" spans="1:11" s="2" customFormat="1">
       <c r="A59" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="4"/>
@@ -2341,13 +2374,13 @@
     </row>
     <row r="60" spans="1:11" s="2" customFormat="1">
       <c r="A60" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
@@ -2360,13 +2393,13 @@
     </row>
     <row r="61" spans="1:11" s="2" customFormat="1">
       <c r="A61" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="4"/>
@@ -2379,13 +2412,13 @@
     </row>
     <row r="62" spans="1:11" s="2" customFormat="1">
       <c r="A62" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="C62" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>199</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
@@ -2398,13 +2431,13 @@
     </row>
     <row r="63" spans="1:11" s="2" customFormat="1">
       <c r="A63" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="C63" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
@@ -2417,13 +2450,13 @@
     </row>
     <row r="64" spans="1:11" s="2" customFormat="1">
       <c r="A64" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>182</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
@@ -2436,13 +2469,13 @@
     </row>
     <row r="65" spans="1:11" s="2" customFormat="1">
       <c r="A65" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
@@ -2455,13 +2488,13 @@
     </row>
     <row r="66" spans="1:11" s="2" customFormat="1">
       <c r="A66" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
@@ -2474,13 +2507,13 @@
     </row>
     <row r="67" spans="1:11" s="2" customFormat="1">
       <c r="A67" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
@@ -2493,13 +2526,13 @@
     </row>
     <row r="68" spans="1:11" s="2" customFormat="1">
       <c r="A68" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="4"/>
@@ -2512,13 +2545,13 @@
     </row>
     <row r="69" spans="1:11" s="2" customFormat="1">
       <c r="A69" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
@@ -2531,13 +2564,13 @@
     </row>
     <row r="70" spans="1:11" s="2" customFormat="1">
       <c r="A70" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
@@ -2550,13 +2583,13 @@
     </row>
     <row r="71" spans="1:11" s="2" customFormat="1">
       <c r="A71" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="4"/>
@@ -2569,13 +2602,13 @@
     </row>
     <row r="72" spans="1:11" s="2" customFormat="1">
       <c r="A72" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="C72" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>196</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="4"/>
@@ -2588,13 +2621,13 @@
     </row>
     <row r="73" spans="1:11" s="2" customFormat="1">
       <c r="A73" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="C73" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="4"/>
@@ -2607,13 +2640,13 @@
     </row>
     <row r="74" spans="1:11" s="2" customFormat="1">
       <c r="A74" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="C74" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>205</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="4"/>
@@ -2626,13 +2659,13 @@
     </row>
     <row r="75" spans="1:11" s="2" customFormat="1">
       <c r="A75" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B75" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="C75" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>208</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="4"/>
@@ -2645,13 +2678,13 @@
     </row>
     <row r="76" spans="1:11" s="2" customFormat="1">
       <c r="A76" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="C76" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="4"/>
@@ -2664,13 +2697,13 @@
     </row>
     <row r="77" spans="1:11" s="2" customFormat="1">
       <c r="A77" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="C77" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>214</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="4"/>
@@ -2683,13 +2716,13 @@
     </row>
     <row r="78" spans="1:11" s="2" customFormat="1">
       <c r="A78" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="C78" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>217</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="4"/>
@@ -2702,13 +2735,13 @@
     </row>
     <row r="79" spans="1:11" s="2" customFormat="1">
       <c r="A79" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="4"/>
@@ -2721,13 +2754,13 @@
     </row>
     <row r="80" spans="1:11" s="2" customFormat="1">
       <c r="A80" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="4"/>
@@ -2740,13 +2773,13 @@
     </row>
     <row r="81" spans="1:11" s="2" customFormat="1">
       <c r="A81" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="4"/>
@@ -2759,13 +2792,13 @@
     </row>
     <row r="82" spans="1:11" s="2" customFormat="1">
       <c r="A82" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="C82" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>229</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="4"/>
@@ -2778,13 +2811,13 @@
     </row>
     <row r="83" spans="1:11" s="2" customFormat="1">
       <c r="A83" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B83" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="C83" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="4"/>
@@ -2797,13 +2830,13 @@
     </row>
     <row r="84" spans="1:11" s="2" customFormat="1">
       <c r="A84" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="4"/>
@@ -2815,9 +2848,15 @@
       <c r="K84" s="11"/>
     </row>
     <row r="85" spans="1:11" s="2" customFormat="1">
-      <c r="A85" s="4"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="4"/>
+      <c r="A85" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>236</v>
+      </c>
       <c r="D85" s="3"/>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -2828,9 +2867,15 @@
       <c r="K85" s="11"/>
     </row>
     <row r="86" spans="1:11" s="2" customFormat="1">
-      <c r="A86" s="4"/>
-      <c r="B86" s="7"/>
-      <c r="C86" s="4"/>
+      <c r="A86" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>239</v>
+      </c>
       <c r="D86" s="3"/>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -2841,9 +2886,15 @@
       <c r="K86" s="11"/>
     </row>
     <row r="87" spans="1:11" s="2" customFormat="1">
-      <c r="A87" s="4"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="4"/>
+      <c r="A87" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>242</v>
+      </c>
       <c r="D87" s="3"/>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -2854,9 +2905,15 @@
       <c r="K87" s="11"/>
     </row>
     <row r="88" spans="1:11" s="2" customFormat="1">
-      <c r="A88" s="4"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="4"/>
+      <c r="A88" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>246</v>
+      </c>
       <c r="D88" s="3"/>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>

</xml_diff>

<commit_message>
[Profile] create page update profile & order history (UI, data & fake API)
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047C78DB-5AB1-464F-BCC1-D9A241957035}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C29BAFD-A61A-4D94-87DB-CF149C0EC9C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$674</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$690</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="383">
   <si>
     <t>EN</t>
   </si>
@@ -359,51 +359,9 @@
     <t>txt_area</t>
   </si>
   <si>
-    <t>Khu vực</t>
-  </si>
-  <si>
     <t>Area</t>
   </si>
   <si>
-    <t>txt_district_1</t>
-  </si>
-  <si>
-    <t>txt_district_2</t>
-  </si>
-  <si>
-    <t>txt_district_3</t>
-  </si>
-  <si>
-    <t>txt_district_4</t>
-  </si>
-  <si>
-    <t>txt_district_5</t>
-  </si>
-  <si>
-    <t>txt_district_6</t>
-  </si>
-  <si>
-    <t>txt_district_7</t>
-  </si>
-  <si>
-    <t>txt_district_8</t>
-  </si>
-  <si>
-    <t>txt_district_9</t>
-  </si>
-  <si>
-    <t>txt_district_10</t>
-  </si>
-  <si>
-    <t>txt_district_11</t>
-  </si>
-  <si>
-    <t>txt_district_12</t>
-  </si>
-  <si>
-    <t>txt_district_13</t>
-  </si>
-  <si>
     <t>Quận 1</t>
   </si>
   <si>
@@ -509,36 +467,6 @@
     <t>Nhà Bè</t>
   </si>
   <si>
-    <t>txt_district_14</t>
-  </si>
-  <si>
-    <t>txt_district_15</t>
-  </si>
-  <si>
-    <t>txt_district_16</t>
-  </si>
-  <si>
-    <t>txt_district_17</t>
-  </si>
-  <si>
-    <t>txt_district_18</t>
-  </si>
-  <si>
-    <t>txt_district_19</t>
-  </si>
-  <si>
-    <t>txt_district_20</t>
-  </si>
-  <si>
-    <t>txt_district_21</t>
-  </si>
-  <si>
-    <t>txt_district_22</t>
-  </si>
-  <si>
-    <t>txt_district_23</t>
-  </si>
-  <si>
     <t>Phu Nhuan</t>
   </si>
   <si>
@@ -629,9 +557,6 @@
     <t>No search results found!</t>
   </si>
   <si>
-    <t>txt_district_24</t>
-  </si>
-  <si>
     <t>Gò vấp</t>
   </si>
   <si>
@@ -780,6 +705,489 @@
   </si>
   <si>
     <t>Payment methods</t>
+  </si>
+  <si>
+    <t>txt_district_0_1</t>
+  </si>
+  <si>
+    <t>txt_district_0_2</t>
+  </si>
+  <si>
+    <t>txt_district_0_3</t>
+  </si>
+  <si>
+    <t>txt_district_0_4</t>
+  </si>
+  <si>
+    <t>txt_district_0_5</t>
+  </si>
+  <si>
+    <t>txt_district_0_6</t>
+  </si>
+  <si>
+    <t>txt_district_0_7</t>
+  </si>
+  <si>
+    <t>txt_district_0_8</t>
+  </si>
+  <si>
+    <t>txt_district_0_9</t>
+  </si>
+  <si>
+    <t>txt_district_0_10</t>
+  </si>
+  <si>
+    <t>txt_district_0_11</t>
+  </si>
+  <si>
+    <t>txt_district_0_12</t>
+  </si>
+  <si>
+    <t>txt_district_0_13</t>
+  </si>
+  <si>
+    <t>txt_district_0_14</t>
+  </si>
+  <si>
+    <t>txt_district_0_15</t>
+  </si>
+  <si>
+    <t>txt_district_0_16</t>
+  </si>
+  <si>
+    <t>txt_district_0_17</t>
+  </si>
+  <si>
+    <t>txt_district_0_18</t>
+  </si>
+  <si>
+    <t>txt_district_0_19</t>
+  </si>
+  <si>
+    <t>txt_district_0_21</t>
+  </si>
+  <si>
+    <t>txt_district_0_20</t>
+  </si>
+  <si>
+    <t>txt_district_0_22</t>
+  </si>
+  <si>
+    <t>txt_district_0_23</t>
+  </si>
+  <si>
+    <t>txt_district_0_24</t>
+  </si>
+  <si>
+    <t>txt_district_1_1</t>
+  </si>
+  <si>
+    <t>txt_district_1_2</t>
+  </si>
+  <si>
+    <t>txt_district_1_3</t>
+  </si>
+  <si>
+    <t>txt_district_1_4</t>
+  </si>
+  <si>
+    <t>txt_district_1_5</t>
+  </si>
+  <si>
+    <t>txt_district_1_6</t>
+  </si>
+  <si>
+    <t>txt_district_1_7</t>
+  </si>
+  <si>
+    <t>txt_district_1_8</t>
+  </si>
+  <si>
+    <t>txt_district_1_9</t>
+  </si>
+  <si>
+    <t>txt_district_1_10</t>
+  </si>
+  <si>
+    <t>txt_district_1_11</t>
+  </si>
+  <si>
+    <t>txt_district_1_12</t>
+  </si>
+  <si>
+    <t>txt_district_1_13</t>
+  </si>
+  <si>
+    <t>txt_district_1_14</t>
+  </si>
+  <si>
+    <t>txt_district_1_15</t>
+  </si>
+  <si>
+    <t>Ba Đình</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cầu Giấy </t>
+  </si>
+  <si>
+    <t>Đống Đa</t>
+  </si>
+  <si>
+    <t>Hà Đông</t>
+  </si>
+  <si>
+    <t>Hai Bà Trưng</t>
+  </si>
+  <si>
+    <t>Hoàn Kiếm</t>
+  </si>
+  <si>
+    <t>Hoàng Mai</t>
+  </si>
+  <si>
+    <t>Long Biên</t>
+  </si>
+  <si>
+    <t>Tây Hồ</t>
+  </si>
+  <si>
+    <t>Thanh Xuân</t>
+  </si>
+  <si>
+    <t>Gia Lâm</t>
+  </si>
+  <si>
+    <t>Hoài Đức</t>
+  </si>
+  <si>
+    <t>Thanh Trì</t>
+  </si>
+  <si>
+    <t>Thường Tín</t>
+  </si>
+  <si>
+    <t>Bắc Tử Liêm</t>
+  </si>
+  <si>
+    <t>Nam Tử Liêm</t>
+  </si>
+  <si>
+    <t>Cau Giay</t>
+  </si>
+  <si>
+    <t>Dong Da</t>
+  </si>
+  <si>
+    <t>Ha Dong</t>
+  </si>
+  <si>
+    <t>Hai Ba Trung</t>
+  </si>
+  <si>
+    <t>Hoan Kiem</t>
+  </si>
+  <si>
+    <t>Hoang Mai</t>
+  </si>
+  <si>
+    <t>Long Bien</t>
+  </si>
+  <si>
+    <t>Tay Ho</t>
+  </si>
+  <si>
+    <t>Thanh Xuan</t>
+  </si>
+  <si>
+    <t>Gia Lam</t>
+  </si>
+  <si>
+    <t>Hoai Duc</t>
+  </si>
+  <si>
+    <t>Thanh Tri</t>
+  </si>
+  <si>
+    <t>Ba Dinh</t>
+  </si>
+  <si>
+    <t>Thuong Tin</t>
+  </si>
+  <si>
+    <t>Bac Tu Liem</t>
+  </si>
+  <si>
+    <t>Nam Tu Liem</t>
+  </si>
+  <si>
+    <t>txt_district_1_16</t>
+  </si>
+  <si>
+    <t>txt_gender_0</t>
+  </si>
+  <si>
+    <t>txt_gender_1</t>
+  </si>
+  <si>
+    <t>txt_gender_2</t>
+  </si>
+  <si>
+    <t>Khác</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>txt_order_status_0</t>
+  </si>
+  <si>
+    <t>txt_order_status_1</t>
+  </si>
+  <si>
+    <t>txt_order_status_2</t>
+  </si>
+  <si>
+    <t>txt_order_status_3</t>
+  </si>
+  <si>
+    <t>txt_order_status_4</t>
+  </si>
+  <si>
+    <t>Đã giao</t>
+  </si>
+  <si>
+    <t>Đang xử lý</t>
+  </si>
+  <si>
+    <t>Đang giao</t>
+  </si>
+  <si>
+    <t>Đã hủy</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
+    <t>Delivering</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>txt_status</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>txt_from_day</t>
+  </si>
+  <si>
+    <t>txt_to_day</t>
+  </si>
+  <si>
+    <t>Từ ngày</t>
+  </si>
+  <si>
+    <t>Đến ngày</t>
+  </si>
+  <si>
+    <t>From date</t>
+  </si>
+  <si>
+    <t>To date</t>
+  </si>
+  <si>
+    <t>text_search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm </t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>txt_total</t>
+  </si>
+  <si>
+    <t>Tổng cộng</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>txt_order</t>
+  </si>
+  <si>
+    <t>Đơn hàng</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>txt_stt</t>
+  </si>
+  <si>
+    <t>txt_order_code</t>
+  </si>
+  <si>
+    <t>txt_time</t>
+  </si>
+  <si>
+    <t>Địa diểm</t>
+  </si>
+  <si>
+    <t>txt_total_money</t>
+  </si>
+  <si>
+    <t>txt_reorder</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Mã đặt hàng</t>
+  </si>
+  <si>
+    <t>Thời gian</t>
+  </si>
+  <si>
+    <t>Tổng tiền</t>
+  </si>
+  <si>
+    <t>Đặt lại</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Order code</t>
+  </si>
+  <si>
+    <t>Total money</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Re-order</t>
+  </si>
+  <si>
+    <t>txt_profile_info</t>
+  </si>
+  <si>
+    <t>txt_update</t>
+  </si>
+  <si>
+    <t>txt_address_info</t>
+  </si>
+  <si>
+    <t>txt_personal_info</t>
+  </si>
+  <si>
+    <t>txt_fullname</t>
+  </si>
+  <si>
+    <t>txt_gender</t>
+  </si>
+  <si>
+    <t>txt_manage_phone</t>
+  </si>
+  <si>
+    <t>txt_phone_vertified</t>
+  </si>
+  <si>
+    <t>Thông tin người dùng</t>
+  </si>
+  <si>
+    <t>Cập nhập</t>
+  </si>
+  <si>
+    <t>Thông tin địa chỉ</t>
+  </si>
+  <si>
+    <t>Thông tin cá nhân</t>
+  </si>
+  <si>
+    <t>Họ tên</t>
+  </si>
+  <si>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>Quản lý số điện thoại</t>
+  </si>
+  <si>
+    <t>số điện thoại đã xác thực</t>
+  </si>
+  <si>
+    <t>User Information</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Fullname</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Address information</t>
+  </si>
+  <si>
+    <t>Personal information</t>
+  </si>
+  <si>
+    <t>Phone number management</t>
+  </si>
+  <si>
+    <t>Phone number is authenticated</t>
+  </si>
+  <si>
+    <t>txt_password</t>
+  </si>
+  <si>
+    <t>Mật khẩu</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>txt_save</t>
+  </si>
+  <si>
+    <t>Lưu thay đổi</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>txt_cancel</t>
+  </si>
+  <si>
+    <t>Hủy</t>
+  </si>
+  <si>
+    <t>Cancel</t>
   </si>
 </sst>
 </file>
@@ -1225,13 +1633,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K1083"/>
+  <dimension ref="A1:K1099"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C95" sqref="C95"/>
+      <selection pane="bottomRight" activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -1408,7 +1816,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>23</v>
@@ -1959,10 +2367,10 @@
         <v>105</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
@@ -1975,13 +2383,13 @@
     </row>
     <row r="39" spans="1:11" s="2" customFormat="1">
       <c r="A39" s="4" t="s">
-        <v>108</v>
+        <v>222</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
@@ -1994,13 +2402,13 @@
     </row>
     <row r="40" spans="1:11" s="2" customFormat="1">
       <c r="A40" s="4" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
@@ -2013,13 +2421,13 @@
     </row>
     <row r="41" spans="1:11" s="2" customFormat="1">
       <c r="A41" s="4" t="s">
-        <v>110</v>
+        <v>224</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
@@ -2032,13 +2440,13 @@
     </row>
     <row r="42" spans="1:11" s="2" customFormat="1">
       <c r="A42" s="4" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
@@ -2051,13 +2459,13 @@
     </row>
     <row r="43" spans="1:11" s="2" customFormat="1">
       <c r="A43" s="4" t="s">
-        <v>112</v>
+        <v>226</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
@@ -2070,13 +2478,13 @@
     </row>
     <row r="44" spans="1:11" s="2" customFormat="1">
       <c r="A44" s="4" t="s">
-        <v>113</v>
+        <v>227</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
@@ -2089,13 +2497,13 @@
     </row>
     <row r="45" spans="1:11" s="2" customFormat="1">
       <c r="A45" s="4" t="s">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
@@ -2108,13 +2516,13 @@
     </row>
     <row r="46" spans="1:11" s="2" customFormat="1">
       <c r="A46" s="4" t="s">
-        <v>115</v>
+        <v>229</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
@@ -2127,13 +2535,13 @@
     </row>
     <row r="47" spans="1:11" s="2" customFormat="1">
       <c r="A47" s="4" t="s">
-        <v>116</v>
+        <v>230</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
@@ -2146,13 +2554,13 @@
     </row>
     <row r="48" spans="1:11" s="2" customFormat="1">
       <c r="A48" s="4" t="s">
-        <v>117</v>
+        <v>231</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
@@ -2165,13 +2573,13 @@
     </row>
     <row r="49" spans="1:11" s="2" customFormat="1">
       <c r="A49" s="4" t="s">
-        <v>118</v>
+        <v>232</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="4"/>
@@ -2184,13 +2592,13 @@
     </row>
     <row r="50" spans="1:11" s="2" customFormat="1">
       <c r="A50" s="4" t="s">
-        <v>119</v>
+        <v>233</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="4"/>
@@ -2203,13 +2611,13 @@
     </row>
     <row r="51" spans="1:11" s="2" customFormat="1">
       <c r="A51" s="4" t="s">
-        <v>120</v>
+        <v>234</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="4"/>
@@ -2222,13 +2630,13 @@
     </row>
     <row r="52" spans="1:11" s="2" customFormat="1">
       <c r="A52" s="4" t="s">
-        <v>156</v>
+        <v>235</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
@@ -2241,13 +2649,13 @@
     </row>
     <row r="53" spans="1:11" s="2" customFormat="1">
       <c r="A53" s="4" t="s">
-        <v>157</v>
+        <v>236</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="4"/>
@@ -2260,13 +2668,13 @@
     </row>
     <row r="54" spans="1:11" s="2" customFormat="1">
       <c r="A54" s="4" t="s">
-        <v>158</v>
+        <v>237</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="4"/>
@@ -2279,13 +2687,13 @@
     </row>
     <row r="55" spans="1:11" s="2" customFormat="1">
       <c r="A55" s="4" t="s">
-        <v>159</v>
+        <v>238</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="4"/>
@@ -2298,13 +2706,13 @@
     </row>
     <row r="56" spans="1:11" s="2" customFormat="1">
       <c r="A56" s="4" t="s">
-        <v>160</v>
+        <v>239</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="4"/>
@@ -2317,13 +2725,13 @@
     </row>
     <row r="57" spans="1:11" s="2" customFormat="1">
       <c r="A57" s="4" t="s">
-        <v>161</v>
+        <v>240</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="4"/>
@@ -2336,13 +2744,13 @@
     </row>
     <row r="58" spans="1:11" s="2" customFormat="1">
       <c r="A58" s="4" t="s">
-        <v>162</v>
+        <v>242</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="4"/>
@@ -2355,13 +2763,13 @@
     </row>
     <row r="59" spans="1:11" s="2" customFormat="1">
       <c r="A59" s="4" t="s">
-        <v>163</v>
+        <v>241</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="4"/>
@@ -2374,13 +2782,13 @@
     </row>
     <row r="60" spans="1:11" s="2" customFormat="1">
       <c r="A60" s="4" t="s">
-        <v>164</v>
+        <v>243</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
@@ -2393,13 +2801,13 @@
     </row>
     <row r="61" spans="1:11" s="2" customFormat="1">
       <c r="A61" s="4" t="s">
-        <v>165</v>
+        <v>244</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="4"/>
@@ -2412,13 +2820,13 @@
     </row>
     <row r="62" spans="1:11" s="2" customFormat="1">
       <c r="A62" s="4" t="s">
-        <v>196</v>
+        <v>245</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
@@ -2431,13 +2839,13 @@
     </row>
     <row r="63" spans="1:11" s="2" customFormat="1">
       <c r="A63" s="4" t="s">
-        <v>177</v>
+        <v>246</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>178</v>
+        <v>261</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>179</v>
+        <v>289</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
@@ -2450,13 +2858,13 @@
     </row>
     <row r="64" spans="1:11" s="2" customFormat="1">
       <c r="A64" s="4" t="s">
-        <v>180</v>
+        <v>247</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>192</v>
+        <v>262</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>181</v>
+        <v>277</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
@@ -2469,13 +2877,13 @@
     </row>
     <row r="65" spans="1:11" s="2" customFormat="1">
       <c r="A65" s="4" t="s">
-        <v>183</v>
+        <v>248</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>64</v>
+        <v>263</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>81</v>
+        <v>278</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
@@ -2488,13 +2896,13 @@
     </row>
     <row r="66" spans="1:11" s="2" customFormat="1">
       <c r="A66" s="4" t="s">
-        <v>184</v>
+        <v>249</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>65</v>
+        <v>264</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>82</v>
+        <v>279</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
@@ -2507,13 +2915,13 @@
     </row>
     <row r="67" spans="1:11" s="2" customFormat="1">
       <c r="A67" s="4" t="s">
-        <v>185</v>
+        <v>250</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>189</v>
+        <v>265</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>85</v>
+        <v>280</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
@@ -2526,13 +2934,13 @@
     </row>
     <row r="68" spans="1:11" s="2" customFormat="1">
       <c r="A68" s="4" t="s">
-        <v>186</v>
+        <v>251</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>190</v>
+        <v>266</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>83</v>
+        <v>281</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="4"/>
@@ -2545,13 +2953,13 @@
     </row>
     <row r="69" spans="1:11" s="2" customFormat="1">
       <c r="A69" s="4" t="s">
-        <v>187</v>
+        <v>252</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>73</v>
+        <v>267</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>88</v>
+        <v>282</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
@@ -2564,13 +2972,13 @@
     </row>
     <row r="70" spans="1:11" s="2" customFormat="1">
       <c r="A70" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>182</v>
+        <v>253</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>182</v>
+        <v>283</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
@@ -2583,13 +2991,13 @@
     </row>
     <row r="71" spans="1:11" s="2" customFormat="1">
       <c r="A71" s="4" t="s">
-        <v>191</v>
+        <v>254</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>72</v>
+        <v>269</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>87</v>
+        <v>284</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="4"/>
@@ -2602,13 +3010,13 @@
     </row>
     <row r="72" spans="1:11" s="2" customFormat="1">
       <c r="A72" s="4" t="s">
-        <v>193</v>
+        <v>255</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>194</v>
+        <v>270</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>195</v>
+        <v>285</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="4"/>
@@ -2621,13 +3029,13 @@
     </row>
     <row r="73" spans="1:11" s="2" customFormat="1">
       <c r="A73" s="4" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>200</v>
+        <v>271</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>201</v>
+        <v>286</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="4"/>
@@ -2640,13 +3048,13 @@
     </row>
     <row r="74" spans="1:11" s="2" customFormat="1">
       <c r="A74" s="4" t="s">
-        <v>202</v>
+        <v>257</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>203</v>
+        <v>272</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>204</v>
+        <v>287</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="4"/>
@@ -2659,13 +3067,13 @@
     </row>
     <row r="75" spans="1:11" s="2" customFormat="1">
       <c r="A75" s="4" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>206</v>
+        <v>273</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="4"/>
@@ -2678,13 +3086,13 @@
     </row>
     <row r="76" spans="1:11" s="2" customFormat="1">
       <c r="A76" s="4" t="s">
-        <v>208</v>
+        <v>259</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>209</v>
+        <v>274</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>210</v>
+        <v>290</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="4"/>
@@ -2697,13 +3105,13 @@
     </row>
     <row r="77" spans="1:11" s="2" customFormat="1">
       <c r="A77" s="4" t="s">
-        <v>211</v>
+        <v>260</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>212</v>
+        <v>275</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>213</v>
+        <v>291</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="4"/>
@@ -2716,13 +3124,13 @@
     </row>
     <row r="78" spans="1:11" s="2" customFormat="1">
       <c r="A78" s="4" t="s">
-        <v>214</v>
+        <v>293</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>215</v>
+        <v>276</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>216</v>
+        <v>292</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="4"/>
@@ -2735,13 +3143,13 @@
     </row>
     <row r="79" spans="1:11" s="2" customFormat="1">
       <c r="A79" s="4" t="s">
-        <v>217</v>
+        <v>153</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>220</v>
+        <v>154</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>223</v>
+        <v>155</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="4"/>
@@ -2754,13 +3162,13 @@
     </row>
     <row r="80" spans="1:11" s="2" customFormat="1">
       <c r="A80" s="4" t="s">
-        <v>218</v>
+        <v>156</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>221</v>
+        <v>168</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>224</v>
+        <v>157</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="4"/>
@@ -2773,13 +3181,13 @@
     </row>
     <row r="81" spans="1:11" s="2" customFormat="1">
       <c r="A81" s="4" t="s">
-        <v>219</v>
+        <v>159</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>222</v>
+        <v>64</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>225</v>
+        <v>81</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="4"/>
@@ -2792,13 +3200,13 @@
     </row>
     <row r="82" spans="1:11" s="2" customFormat="1">
       <c r="A82" s="4" t="s">
-        <v>226</v>
+        <v>160</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>227</v>
+        <v>65</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>228</v>
+        <v>82</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="4"/>
@@ -2811,13 +3219,13 @@
     </row>
     <row r="83" spans="1:11" s="2" customFormat="1">
       <c r="A83" s="4" t="s">
-        <v>229</v>
+        <v>161</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>230</v>
+        <v>165</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>233</v>
+        <v>85</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="4"/>
@@ -2830,13 +3238,13 @@
     </row>
     <row r="84" spans="1:11" s="2" customFormat="1">
       <c r="A84" s="4" t="s">
-        <v>232</v>
+        <v>162</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>231</v>
+        <v>166</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>234</v>
+        <v>83</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="4"/>
@@ -2849,13 +3257,13 @@
     </row>
     <row r="85" spans="1:11" s="2" customFormat="1">
       <c r="A85" s="4" t="s">
-        <v>235</v>
+        <v>163</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>203</v>
+        <v>73</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>236</v>
+        <v>88</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="4"/>
@@ -2868,13 +3276,13 @@
     </row>
     <row r="86" spans="1:11" s="2" customFormat="1">
       <c r="A86" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>238</v>
+        <v>164</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>239</v>
+        <v>158</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="4"/>
@@ -2887,13 +3295,13 @@
     </row>
     <row r="87" spans="1:11" s="2" customFormat="1">
       <c r="A87" s="4" t="s">
-        <v>240</v>
+        <v>167</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>241</v>
+        <v>72</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>242</v>
+        <v>87</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="4"/>
@@ -2906,13 +3314,13 @@
     </row>
     <row r="88" spans="1:11" s="2" customFormat="1">
       <c r="A88" s="4" t="s">
-        <v>244</v>
+        <v>169</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>245</v>
+        <v>170</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>246</v>
+        <v>171</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="4"/>
@@ -2924,9 +3332,15 @@
       <c r="K88" s="11"/>
     </row>
     <row r="89" spans="1:11" s="2" customFormat="1">
-      <c r="A89" s="4"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="4"/>
+      <c r="A89" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>176</v>
+      </c>
       <c r="D89" s="3"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -2937,9 +3351,15 @@
       <c r="K89" s="11"/>
     </row>
     <row r="90" spans="1:11" s="2" customFormat="1">
-      <c r="A90" s="4"/>
-      <c r="B90" s="7"/>
-      <c r="C90" s="4"/>
+      <c r="A90" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>179</v>
+      </c>
       <c r="D90" s="3"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
@@ -2950,9 +3370,15 @@
       <c r="K90" s="11"/>
     </row>
     <row r="91" spans="1:11" s="2" customFormat="1">
-      <c r="A91" s="4"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="4"/>
+      <c r="A91" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="D91" s="3"/>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
@@ -2963,9 +3389,15 @@
       <c r="K91" s="11"/>
     </row>
     <row r="92" spans="1:11" s="2" customFormat="1">
-      <c r="A92" s="4"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="4"/>
+      <c r="A92" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="D92" s="3"/>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -2976,9 +3408,15 @@
       <c r="K92" s="11"/>
     </row>
     <row r="93" spans="1:11" s="2" customFormat="1">
-      <c r="A93" s="4"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="4"/>
+      <c r="A93" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="D93" s="3"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
@@ -2989,9 +3427,15 @@
       <c r="K93" s="11"/>
     </row>
     <row r="94" spans="1:11" s="2" customFormat="1">
-      <c r="A94" s="4"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="4"/>
+      <c r="A94" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="D94" s="3"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
@@ -3002,9 +3446,15 @@
       <c r="K94" s="11"/>
     </row>
     <row r="95" spans="1:11" s="2" customFormat="1">
-      <c r="A95" s="4"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="4"/>
+      <c r="A95" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="D95" s="3"/>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
@@ -3015,9 +3465,15 @@
       <c r="K95" s="11"/>
     </row>
     <row r="96" spans="1:11" s="2" customFormat="1">
-      <c r="A96" s="4"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="4"/>
+      <c r="A96" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>199</v>
+      </c>
       <c r="D96" s="3"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
@@ -3028,9 +3484,15 @@
       <c r="K96" s="11"/>
     </row>
     <row r="97" spans="1:11" s="2" customFormat="1">
-      <c r="A97" s="4"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="4"/>
+      <c r="A97" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="D97" s="3"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
@@ -3041,9 +3503,15 @@
       <c r="K97" s="11"/>
     </row>
     <row r="98" spans="1:11" s="2" customFormat="1">
-      <c r="A98" s="4"/>
-      <c r="B98" s="7"/>
-      <c r="C98" s="4"/>
+      <c r="A98" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>203</v>
+      </c>
       <c r="D98" s="3"/>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
@@ -3054,9 +3522,15 @@
       <c r="K98" s="11"/>
     </row>
     <row r="99" spans="1:11" s="2" customFormat="1">
-      <c r="A99" s="4"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="4"/>
+      <c r="A99" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>208</v>
+      </c>
       <c r="D99" s="3"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
@@ -3067,9 +3541,15 @@
       <c r="K99" s="11"/>
     </row>
     <row r="100" spans="1:11" s="2" customFormat="1">
-      <c r="A100" s="4"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="4"/>
+      <c r="A100" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>209</v>
+      </c>
       <c r="D100" s="3"/>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
@@ -3080,9 +3560,15 @@
       <c r="K100" s="11"/>
     </row>
     <row r="101" spans="1:11" s="2" customFormat="1">
-      <c r="A101" s="4"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="4"/>
+      <c r="A101" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="D101" s="3"/>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
@@ -3093,9 +3579,15 @@
       <c r="K101" s="11"/>
     </row>
     <row r="102" spans="1:11" s="2" customFormat="1">
-      <c r="A102" s="4"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="4"/>
+      <c r="A102" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="D102" s="3"/>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
@@ -3106,9 +3598,15 @@
       <c r="K102" s="11"/>
     </row>
     <row r="103" spans="1:11" s="2" customFormat="1">
-      <c r="A103" s="4"/>
-      <c r="B103" s="7"/>
-      <c r="C103" s="4"/>
+      <c r="A103" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="D103" s="3"/>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
@@ -3119,9 +3617,15 @@
       <c r="K103" s="11"/>
     </row>
     <row r="104" spans="1:11" s="2" customFormat="1">
-      <c r="A104" s="4"/>
-      <c r="B104" s="7"/>
-      <c r="C104" s="4"/>
+      <c r="A104" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="D104" s="3"/>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -3132,9 +3636,15 @@
       <c r="K104" s="11"/>
     </row>
     <row r="105" spans="1:11" s="2" customFormat="1">
-      <c r="A105" s="4"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="4"/>
+      <c r="A105" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>300</v>
+      </c>
       <c r="D105" s="3"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -3145,9 +3655,15 @@
       <c r="K105" s="11"/>
     </row>
     <row r="106" spans="1:11" s="2" customFormat="1">
-      <c r="A106" s="4"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="4"/>
+      <c r="A106" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>301</v>
+      </c>
       <c r="D106" s="3"/>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
@@ -3158,9 +3674,15 @@
       <c r="K106" s="11"/>
     </row>
     <row r="107" spans="1:11" s="2" customFormat="1">
-      <c r="A107" s="4"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="4"/>
+      <c r="A107" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>302</v>
+      </c>
       <c r="D107" s="3"/>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
@@ -3171,9 +3693,15 @@
       <c r="K107" s="11"/>
     </row>
     <row r="108" spans="1:11" s="2" customFormat="1">
-      <c r="A108" s="4"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="4"/>
+      <c r="A108" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="D108" s="3"/>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
@@ -3184,9 +3712,15 @@
       <c r="K108" s="11"/>
     </row>
     <row r="109" spans="1:11" s="2" customFormat="1">
-      <c r="A109" s="4"/>
-      <c r="B109" s="7"/>
-      <c r="C109" s="4"/>
+      <c r="A109" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>312</v>
+      </c>
       <c r="D109" s="3"/>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
@@ -3197,9 +3731,15 @@
       <c r="K109" s="11"/>
     </row>
     <row r="110" spans="1:11" s="2" customFormat="1">
-      <c r="A110" s="4"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="4"/>
+      <c r="A110" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>313</v>
+      </c>
       <c r="D110" s="3"/>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
@@ -3210,9 +3750,15 @@
       <c r="K110" s="11"/>
     </row>
     <row r="111" spans="1:11" s="2" customFormat="1">
-      <c r="A111" s="4"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="4"/>
+      <c r="A111" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>314</v>
+      </c>
       <c r="D111" s="3"/>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
@@ -3223,9 +3769,15 @@
       <c r="K111" s="11"/>
     </row>
     <row r="112" spans="1:11" s="2" customFormat="1">
-      <c r="A112" s="4"/>
-      <c r="B112" s="7"/>
-      <c r="C112" s="4"/>
+      <c r="A112" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>315</v>
+      </c>
       <c r="D112" s="3"/>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
@@ -3236,9 +3788,15 @@
       <c r="K112" s="11"/>
     </row>
     <row r="113" spans="1:11" s="2" customFormat="1">
-      <c r="A113" s="4"/>
-      <c r="B113" s="7"/>
-      <c r="C113" s="4"/>
+      <c r="A113" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>318</v>
+      </c>
       <c r="D113" s="3"/>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
@@ -3249,9 +3807,15 @@
       <c r="K113" s="11"/>
     </row>
     <row r="114" spans="1:11" s="2" customFormat="1">
-      <c r="A114" s="4"/>
-      <c r="B114" s="7"/>
-      <c r="C114" s="4"/>
+      <c r="A114" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>323</v>
+      </c>
       <c r="D114" s="3"/>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
@@ -3262,9 +3826,15 @@
       <c r="K114" s="11"/>
     </row>
     <row r="115" spans="1:11" s="2" customFormat="1">
-      <c r="A115" s="4"/>
-      <c r="B115" s="7"/>
-      <c r="C115" s="4"/>
+      <c r="A115" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>324</v>
+      </c>
       <c r="D115" s="3"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
@@ -3275,9 +3845,15 @@
       <c r="K115" s="11"/>
     </row>
     <row r="116" spans="1:11" s="2" customFormat="1">
-      <c r="A116" s="4"/>
-      <c r="B116" s="7"/>
-      <c r="C116" s="4"/>
+      <c r="A116" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>327</v>
+      </c>
       <c r="D116" s="3"/>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -3288,9 +3864,15 @@
       <c r="K116" s="11"/>
     </row>
     <row r="117" spans="1:11" s="2" customFormat="1">
-      <c r="A117" s="4"/>
-      <c r="B117" s="7"/>
-      <c r="C117" s="4"/>
+      <c r="A117" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>330</v>
+      </c>
       <c r="D117" s="3"/>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
@@ -3301,9 +3883,15 @@
       <c r="K117" s="11"/>
     </row>
     <row r="118" spans="1:11" s="2" customFormat="1">
-      <c r="A118" s="4"/>
-      <c r="B118" s="7"/>
-      <c r="C118" s="4"/>
+      <c r="A118" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>333</v>
+      </c>
       <c r="D118" s="3"/>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
@@ -3314,9 +3902,15 @@
       <c r="K118" s="11"/>
     </row>
     <row r="119" spans="1:11" s="2" customFormat="1">
-      <c r="A119" s="4"/>
-      <c r="B119" s="7"/>
-      <c r="C119" s="4"/>
+      <c r="A119" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>345</v>
+      </c>
       <c r="D119" s="3"/>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
@@ -3327,9 +3921,15 @@
       <c r="K119" s="11"/>
     </row>
     <row r="120" spans="1:11" s="2" customFormat="1">
-      <c r="A120" s="4"/>
-      <c r="B120" s="7"/>
-      <c r="C120" s="4"/>
+      <c r="A120" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="D120" s="3"/>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
@@ -3340,9 +3940,15 @@
       <c r="K120" s="11"/>
     </row>
     <row r="121" spans="1:11" s="2" customFormat="1">
-      <c r="A121" s="4"/>
-      <c r="B121" s="7"/>
-      <c r="C121" s="4"/>
+      <c r="A121" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>348</v>
+      </c>
       <c r="D121" s="3"/>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
@@ -3353,9 +3959,15 @@
       <c r="K121" s="11"/>
     </row>
     <row r="122" spans="1:11" s="2" customFormat="1">
-      <c r="A122" s="4"/>
-      <c r="B122" s="7"/>
-      <c r="C122" s="4"/>
+      <c r="A122" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>347</v>
+      </c>
       <c r="D122" s="3"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
@@ -3366,9 +3978,15 @@
       <c r="K122" s="11"/>
     </row>
     <row r="123" spans="1:11" s="2" customFormat="1">
-      <c r="A123" s="4"/>
-      <c r="B123" s="7"/>
-      <c r="C123" s="4"/>
+      <c r="A123" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>349</v>
+      </c>
       <c r="D123" s="3"/>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
@@ -3379,9 +3997,15 @@
       <c r="K123" s="11"/>
     </row>
     <row r="124" spans="1:11" s="2" customFormat="1">
-      <c r="A124" s="4"/>
-      <c r="B124" s="7"/>
-      <c r="C124" s="4"/>
+      <c r="A124" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>366</v>
+      </c>
       <c r="D124" s="3"/>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
@@ -3392,9 +4016,15 @@
       <c r="K124" s="11"/>
     </row>
     <row r="125" spans="1:11" s="2" customFormat="1">
-      <c r="A125" s="4"/>
-      <c r="B125" s="7"/>
-      <c r="C125" s="4"/>
+      <c r="A125" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>367</v>
+      </c>
       <c r="D125" s="3"/>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
@@ -3405,9 +4035,15 @@
       <c r="K125" s="11"/>
     </row>
     <row r="126" spans="1:11" s="2" customFormat="1">
-      <c r="A126" s="4"/>
-      <c r="B126" s="7"/>
-      <c r="C126" s="4"/>
+      <c r="A126" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>370</v>
+      </c>
       <c r="D126" s="3"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
@@ -3418,9 +4054,15 @@
       <c r="K126" s="11"/>
     </row>
     <row r="127" spans="1:11" s="2" customFormat="1">
-      <c r="A127" s="4"/>
-      <c r="B127" s="7"/>
-      <c r="C127" s="4"/>
+      <c r="A127" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>371</v>
+      </c>
       <c r="D127" s="3"/>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
@@ -3431,9 +4073,15 @@
       <c r="K127" s="11"/>
     </row>
     <row r="128" spans="1:11" s="2" customFormat="1">
-      <c r="A128" s="4"/>
-      <c r="B128" s="7"/>
-      <c r="C128" s="4"/>
+      <c r="A128" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>368</v>
+      </c>
       <c r="D128" s="3"/>
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
@@ -3444,9 +4092,15 @@
       <c r="K128" s="11"/>
     </row>
     <row r="129" spans="1:11" s="2" customFormat="1">
-      <c r="A129" s="4"/>
-      <c r="B129" s="7"/>
-      <c r="C129" s="4"/>
+      <c r="A129" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>369</v>
+      </c>
       <c r="D129" s="3"/>
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
@@ -3457,9 +4111,15 @@
       <c r="K129" s="11"/>
     </row>
     <row r="130" spans="1:11" s="2" customFormat="1">
-      <c r="A130" s="4"/>
-      <c r="B130" s="7"/>
-      <c r="C130" s="4"/>
+      <c r="A130" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>372</v>
+      </c>
       <c r="D130" s="3"/>
       <c r="E130" s="4"/>
       <c r="F130" s="4"/>
@@ -3470,9 +4130,15 @@
       <c r="K130" s="11"/>
     </row>
     <row r="131" spans="1:11" s="2" customFormat="1">
-      <c r="A131" s="4"/>
-      <c r="B131" s="7"/>
-      <c r="C131" s="4"/>
+      <c r="A131" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>373</v>
+      </c>
       <c r="D131" s="3"/>
       <c r="E131" s="4"/>
       <c r="F131" s="4"/>
@@ -3483,9 +4149,15 @@
       <c r="K131" s="11"/>
     </row>
     <row r="132" spans="1:11" s="2" customFormat="1">
-      <c r="A132" s="4"/>
-      <c r="B132" s="7"/>
-      <c r="C132" s="4"/>
+      <c r="A132" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>376</v>
+      </c>
       <c r="D132" s="3"/>
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
@@ -3496,9 +4168,15 @@
       <c r="K132" s="11"/>
     </row>
     <row r="133" spans="1:11" s="2" customFormat="1">
-      <c r="A133" s="4"/>
-      <c r="B133" s="7"/>
-      <c r="C133" s="4"/>
+      <c r="A133" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>379</v>
+      </c>
       <c r="D133" s="3"/>
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
@@ -3509,9 +4187,15 @@
       <c r="K133" s="11"/>
     </row>
     <row r="134" spans="1:11" s="2" customFormat="1">
-      <c r="A134" s="4"/>
-      <c r="B134" s="7"/>
-      <c r="C134" s="4"/>
+      <c r="A134" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="D134" s="3"/>
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
@@ -15806,28 +16490,236 @@
       <c r="J1079" s="10"/>
       <c r="K1079" s="11"/>
     </row>
-    <row r="1080" spans="1:11">
-      <c r="A1080" s="8"/>
-      <c r="B1080" s="8"/>
-      <c r="C1080" s="8"/>
-    </row>
-    <row r="1081" spans="1:11">
-      <c r="A1081" s="8"/>
-      <c r="B1081" s="8"/>
-      <c r="C1081" s="8"/>
-    </row>
-    <row r="1082" spans="1:11">
-      <c r="A1082" s="8"/>
-      <c r="B1082" s="8"/>
-      <c r="C1082" s="8"/>
-    </row>
-    <row r="1083" spans="1:11">
-      <c r="A1083" s="8"/>
-      <c r="B1083" s="8"/>
-      <c r="C1083" s="8"/>
+    <row r="1080" spans="1:11" s="2" customFormat="1">
+      <c r="A1080" s="4"/>
+      <c r="B1080" s="7"/>
+      <c r="C1080" s="4"/>
+      <c r="D1080" s="3"/>
+      <c r="E1080" s="4"/>
+      <c r="F1080" s="4"/>
+      <c r="G1080" s="4"/>
+      <c r="H1080" s="4"/>
+      <c r="I1080" s="4"/>
+      <c r="J1080" s="10"/>
+      <c r="K1080" s="11"/>
+    </row>
+    <row r="1081" spans="1:11" s="2" customFormat="1">
+      <c r="A1081" s="4"/>
+      <c r="B1081" s="7"/>
+      <c r="C1081" s="4"/>
+      <c r="D1081" s="3"/>
+      <c r="E1081" s="4"/>
+      <c r="F1081" s="4"/>
+      <c r="G1081" s="4"/>
+      <c r="H1081" s="4"/>
+      <c r="I1081" s="4"/>
+      <c r="J1081" s="10"/>
+      <c r="K1081" s="11"/>
+    </row>
+    <row r="1082" spans="1:11" s="2" customFormat="1">
+      <c r="A1082" s="4"/>
+      <c r="B1082" s="7"/>
+      <c r="C1082" s="4"/>
+      <c r="D1082" s="3"/>
+      <c r="E1082" s="4"/>
+      <c r="F1082" s="4"/>
+      <c r="G1082" s="4"/>
+      <c r="H1082" s="4"/>
+      <c r="I1082" s="4"/>
+      <c r="J1082" s="10"/>
+      <c r="K1082" s="11"/>
+    </row>
+    <row r="1083" spans="1:11" s="2" customFormat="1">
+      <c r="A1083" s="4"/>
+      <c r="B1083" s="7"/>
+      <c r="C1083" s="4"/>
+      <c r="D1083" s="3"/>
+      <c r="E1083" s="4"/>
+      <c r="F1083" s="4"/>
+      <c r="G1083" s="4"/>
+      <c r="H1083" s="4"/>
+      <c r="I1083" s="4"/>
+      <c r="J1083" s="10"/>
+      <c r="K1083" s="11"/>
+    </row>
+    <row r="1084" spans="1:11" s="2" customFormat="1">
+      <c r="A1084" s="4"/>
+      <c r="B1084" s="7"/>
+      <c r="C1084" s="4"/>
+      <c r="D1084" s="3"/>
+      <c r="E1084" s="4"/>
+      <c r="F1084" s="4"/>
+      <c r="G1084" s="4"/>
+      <c r="H1084" s="4"/>
+      <c r="I1084" s="4"/>
+      <c r="J1084" s="10"/>
+      <c r="K1084" s="11"/>
+    </row>
+    <row r="1085" spans="1:11" s="2" customFormat="1">
+      <c r="A1085" s="4"/>
+      <c r="B1085" s="7"/>
+      <c r="C1085" s="4"/>
+      <c r="D1085" s="3"/>
+      <c r="E1085" s="4"/>
+      <c r="F1085" s="4"/>
+      <c r="G1085" s="4"/>
+      <c r="H1085" s="4"/>
+      <c r="I1085" s="4"/>
+      <c r="J1085" s="10"/>
+      <c r="K1085" s="11"/>
+    </row>
+    <row r="1086" spans="1:11" s="2" customFormat="1">
+      <c r="A1086" s="4"/>
+      <c r="B1086" s="7"/>
+      <c r="C1086" s="4"/>
+      <c r="D1086" s="3"/>
+      <c r="E1086" s="4"/>
+      <c r="F1086" s="4"/>
+      <c r="G1086" s="4"/>
+      <c r="H1086" s="4"/>
+      <c r="I1086" s="4"/>
+      <c r="J1086" s="10"/>
+      <c r="K1086" s="11"/>
+    </row>
+    <row r="1087" spans="1:11" s="2" customFormat="1">
+      <c r="A1087" s="4"/>
+      <c r="B1087" s="7"/>
+      <c r="C1087" s="4"/>
+      <c r="D1087" s="3"/>
+      <c r="E1087" s="4"/>
+      <c r="F1087" s="4"/>
+      <c r="G1087" s="4"/>
+      <c r="H1087" s="4"/>
+      <c r="I1087" s="4"/>
+      <c r="J1087" s="10"/>
+      <c r="K1087" s="11"/>
+    </row>
+    <row r="1088" spans="1:11" s="2" customFormat="1">
+      <c r="A1088" s="4"/>
+      <c r="B1088" s="7"/>
+      <c r="C1088" s="4"/>
+      <c r="D1088" s="3"/>
+      <c r="E1088" s="4"/>
+      <c r="F1088" s="4"/>
+      <c r="G1088" s="4"/>
+      <c r="H1088" s="4"/>
+      <c r="I1088" s="4"/>
+      <c r="J1088" s="10"/>
+      <c r="K1088" s="11"/>
+    </row>
+    <row r="1089" spans="1:11" s="2" customFormat="1">
+      <c r="A1089" s="4"/>
+      <c r="B1089" s="7"/>
+      <c r="C1089" s="4"/>
+      <c r="D1089" s="3"/>
+      <c r="E1089" s="4"/>
+      <c r="F1089" s="4"/>
+      <c r="G1089" s="4"/>
+      <c r="H1089" s="4"/>
+      <c r="I1089" s="4"/>
+      <c r="J1089" s="10"/>
+      <c r="K1089" s="11"/>
+    </row>
+    <row r="1090" spans="1:11" s="2" customFormat="1">
+      <c r="A1090" s="4"/>
+      <c r="B1090" s="7"/>
+      <c r="C1090" s="4"/>
+      <c r="D1090" s="3"/>
+      <c r="E1090" s="4"/>
+      <c r="F1090" s="4"/>
+      <c r="G1090" s="4"/>
+      <c r="H1090" s="4"/>
+      <c r="I1090" s="4"/>
+      <c r="J1090" s="10"/>
+      <c r="K1090" s="11"/>
+    </row>
+    <row r="1091" spans="1:11" s="2" customFormat="1">
+      <c r="A1091" s="4"/>
+      <c r="B1091" s="7"/>
+      <c r="C1091" s="4"/>
+      <c r="D1091" s="3"/>
+      <c r="E1091" s="4"/>
+      <c r="F1091" s="4"/>
+      <c r="G1091" s="4"/>
+      <c r="H1091" s="4"/>
+      <c r="I1091" s="4"/>
+      <c r="J1091" s="10"/>
+      <c r="K1091" s="11"/>
+    </row>
+    <row r="1092" spans="1:11" s="2" customFormat="1">
+      <c r="A1092" s="4"/>
+      <c r="B1092" s="7"/>
+      <c r="C1092" s="4"/>
+      <c r="D1092" s="3"/>
+      <c r="E1092" s="4"/>
+      <c r="F1092" s="4"/>
+      <c r="G1092" s="4"/>
+      <c r="H1092" s="4"/>
+      <c r="I1092" s="4"/>
+      <c r="J1092" s="10"/>
+      <c r="K1092" s="11"/>
+    </row>
+    <row r="1093" spans="1:11" s="2" customFormat="1">
+      <c r="A1093" s="4"/>
+      <c r="B1093" s="7"/>
+      <c r="C1093" s="4"/>
+      <c r="D1093" s="3"/>
+      <c r="E1093" s="4"/>
+      <c r="F1093" s="4"/>
+      <c r="G1093" s="4"/>
+      <c r="H1093" s="4"/>
+      <c r="I1093" s="4"/>
+      <c r="J1093" s="10"/>
+      <c r="K1093" s="11"/>
+    </row>
+    <row r="1094" spans="1:11" s="2" customFormat="1">
+      <c r="A1094" s="4"/>
+      <c r="B1094" s="7"/>
+      <c r="C1094" s="4"/>
+      <c r="D1094" s="3"/>
+      <c r="E1094" s="4"/>
+      <c r="F1094" s="4"/>
+      <c r="G1094" s="4"/>
+      <c r="H1094" s="4"/>
+      <c r="I1094" s="4"/>
+      <c r="J1094" s="10"/>
+      <c r="K1094" s="11"/>
+    </row>
+    <row r="1095" spans="1:11" s="2" customFormat="1">
+      <c r="A1095" s="4"/>
+      <c r="B1095" s="7"/>
+      <c r="C1095" s="4"/>
+      <c r="D1095" s="3"/>
+      <c r="E1095" s="4"/>
+      <c r="F1095" s="4"/>
+      <c r="G1095" s="4"/>
+      <c r="H1095" s="4"/>
+      <c r="I1095" s="4"/>
+      <c r="J1095" s="10"/>
+      <c r="K1095" s="11"/>
+    </row>
+    <row r="1096" spans="1:11">
+      <c r="A1096" s="8"/>
+      <c r="B1096" s="8"/>
+      <c r="C1096" s="8"/>
+    </row>
+    <row r="1097" spans="1:11">
+      <c r="A1097" s="8"/>
+      <c r="B1097" s="8"/>
+      <c r="C1097" s="8"/>
+    </row>
+    <row r="1098" spans="1:11">
+      <c r="A1098" s="8"/>
+      <c r="B1098" s="8"/>
+      <c r="C1098" s="8"/>
+    </row>
+    <row r="1099" spans="1:11">
+      <c r="A1099" s="8"/>
+      <c r="B1099" s="8"/>
+      <c r="C1099" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I674" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I690" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
change background at home page
</commit_message>
<xml_diff>
--- a/tools/text-wrapper/language_main.xlsx
+++ b/tools/text-wrapper/language_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGame\Now\customer-delivery-food\tools\text-wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C29BAFD-A61A-4D94-87DB-CF149C0EC9C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E3B197-0CD7-493A-AF52-D82110A33D44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="403">
   <si>
     <t>EN</t>
   </si>
@@ -1188,6 +1188,66 @@
   </si>
   <si>
     <t>Cancel</t>
+  </si>
+  <si>
+    <t>txt_collections</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>txt_view_all</t>
+  </si>
+  <si>
+    <t>Xem tất cả</t>
+  </si>
+  <si>
+    <t>txt_nearby</t>
+  </si>
+  <si>
+    <t>Gần đây</t>
+  </si>
+  <si>
+    <t>Nearby</t>
+  </si>
+  <si>
+    <t>txt_top_sales</t>
+  </si>
+  <si>
+    <t>Bán chạy</t>
+  </si>
+  <si>
+    <t>Top sales</t>
+  </si>
+  <si>
+    <t>txt_best_rated</t>
+  </si>
+  <si>
+    <t>Đánh giá</t>
+  </si>
+  <si>
+    <t>Best rated</t>
+  </si>
+  <si>
+    <t>txt_fast</t>
+  </si>
+  <si>
+    <t>Giao nhanh</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>txt_load_more</t>
+  </si>
+  <si>
+    <t>Xem thêm</t>
+  </si>
+  <si>
+    <t>Load more</t>
+  </si>
+  <si>
+    <t>Bộ sưu tập</t>
   </si>
 </sst>
 </file>
@@ -1636,10 +1696,10 @@
   <dimension ref="A1:K1099"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C120" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C134" sqref="C134"/>
+      <selection pane="bottomRight" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -4206,9 +4266,15 @@
       <c r="K134" s="11"/>
     </row>
     <row r="135" spans="1:11" s="2" customFormat="1">
-      <c r="A135" s="4"/>
-      <c r="B135" s="7"/>
-      <c r="C135" s="4"/>
+      <c r="A135" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="D135" s="3"/>
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
@@ -4219,9 +4285,15 @@
       <c r="K135" s="11"/>
     </row>
     <row r="136" spans="1:11" s="2" customFormat="1">
-      <c r="A136" s="4"/>
-      <c r="B136" s="7"/>
-      <c r="C136" s="4"/>
+      <c r="A136" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>386</v>
+      </c>
       <c r="D136" s="3"/>
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
@@ -4232,9 +4304,15 @@
       <c r="K136" s="11"/>
     </row>
     <row r="137" spans="1:11" s="2" customFormat="1">
-      <c r="A137" s="4"/>
-      <c r="B137" s="7"/>
-      <c r="C137" s="4"/>
+      <c r="A137" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>389</v>
+      </c>
       <c r="D137" s="3"/>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
@@ -4245,9 +4323,15 @@
       <c r="K137" s="11"/>
     </row>
     <row r="138" spans="1:11" s="2" customFormat="1">
-      <c r="A138" s="4"/>
-      <c r="B138" s="7"/>
-      <c r="C138" s="4"/>
+      <c r="A138" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>392</v>
+      </c>
       <c r="D138" s="3"/>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
@@ -4258,9 +4342,15 @@
       <c r="K138" s="11"/>
     </row>
     <row r="139" spans="1:11" s="2" customFormat="1">
-      <c r="A139" s="4"/>
-      <c r="B139" s="7"/>
-      <c r="C139" s="4"/>
+      <c r="A139" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>395</v>
+      </c>
       <c r="D139" s="3"/>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
@@ -4271,9 +4361,15 @@
       <c r="K139" s="11"/>
     </row>
     <row r="140" spans="1:11" s="2" customFormat="1">
-      <c r="A140" s="4"/>
-      <c r="B140" s="7"/>
-      <c r="C140" s="4"/>
+      <c r="A140" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>398</v>
+      </c>
       <c r="D140" s="3"/>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
@@ -4284,9 +4380,15 @@
       <c r="K140" s="11"/>
     </row>
     <row r="141" spans="1:11" s="2" customFormat="1">
-      <c r="A141" s="4"/>
-      <c r="B141" s="7"/>
-      <c r="C141" s="4"/>
+      <c r="A141" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>401</v>
+      </c>
       <c r="D141" s="3"/>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>

</xml_diff>